<commit_message>
Add last tweaks to the code before big launch
</commit_message>
<xml_diff>
--- a/Input/AIDS_epidemic.xlsx
+++ b/Input/AIDS_epidemic.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">B-(u*X)-((beta*c*Y*X)/(X+Y+Z+A))</t>
+    <t xml:space="preserve">B-(u*X)-((G*c*Y*X)/(X+Y+Z+A))</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
@@ -58,13 +58,13 @@
     <t xml:space="preserve">u</t>
   </si>
   <si>
-    <t xml:space="preserve">((beta*c*Y*X)/(X+Y+Z+A))-((v+u)*Y)</t>
+    <t xml:space="preserve">((G*c*Y*X)/(X+Y+Z+A))-((v+u)*Y)</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">beta</t>
+    <t xml:space="preserve">G</t>
   </si>
   <si>
     <t xml:space="preserve">((p*v)*Y)-((d+u)*A)</t>
@@ -95,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,11 +116,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,16 +160,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -198,10 +189,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="71.94"/>
@@ -249,7 +240,7 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>